<commit_message>
Cover that tasks Milestone 7
</commit_message>
<xml_diff>
--- a/airport_petty_algorithms/carrier_register/Звіт Jet A-1.xlsx
+++ b/airport_petty_algorithms/carrier_register/Звіт Jet A-1.xlsx
@@ -36,7 +36,7 @@
     <t xml:space="preserve">по руху палива JEТA-1 ПАТ "Укртатнафта" в а/п Львів</t>
   </si>
   <si>
-    <t xml:space="preserve">Дата: 05.09.2021</t>
+    <t xml:space="preserve">Дата: 09.09.2021</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
@@ -235,7 +235,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,6 +243,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,11 +267,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,10 +281,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -367,17 +367,17 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="69.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="50"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -389,7 +389,7 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -400,246 +400,246 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="n">
-        <v>23276</v>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="n">
+        <v>18463</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5" t="n">
-        <v>6381</v>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="n">
+        <v>6720</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="G7" s="8"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="I9" s="9"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7" t="n">
-        <v>30292</v>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8" t="n">
+        <v>11986</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7" t="n">
-        <v>26268</v>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8" t="n">
+        <v>20222</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5" t="n">
+      <c r="B19" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="n">
+      <c r="B20" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="4"/>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="10" t="n">
-        <v>86217</v>
+      <c r="D21" s="6"/>
+      <c r="E21" s="11" t="n">
+        <v>57391</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="11" t="n">
-        <v>61660</v>
+      <c r="D23" s="6"/>
+      <c r="E23" s="12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="10" t="n">
-        <v>57718</v>
+      <c r="D24" s="5"/>
+      <c r="E24" s="11" t="n">
+        <v>310083</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="H41uGY8cT3liP4nd0hZHRtf6CpJhmLptifjVVmiP/GMILinZd0gUbPuw5dDI0lY1Y3sq2DFOzHOyGKBfZ/WdWw==" saltValue="MXyfoaFFaqTyvqiQEgog6w==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>

</xml_diff>